<commit_message>
updated data and expandr
</commit_message>
<xml_diff>
--- a/processed data/explore expandr.xlsx
+++ b/processed data/explore expandr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mygithub\data-indonesia-covid19\processed data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3778BEB3-DB98-4123-9DB1-CCAA80C121BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6AC04C-D676-4C50-9005-7A58E9EB390C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{99997AC6-4747-4E3C-BD2F-4A87F19432B6}"/>
   </bookViews>
@@ -190,10 +190,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>3Tshare_gdp</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>loan_q1_yoy</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -267,6 +263,10 @@
   </si>
   <si>
     <t>province</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TTTshare_gdp</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -321,12 +321,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -647,23 +650,24 @@
   <dimension ref="A1:AC35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2:L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
   <cols>
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" customWidth="1"/>
     <col min="16" max="16" width="10.08203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.08203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.83203125" customWidth="1"/>
-    <col min="22" max="22" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="25" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="26" max="28" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -674,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
         <v>35</v>
@@ -716,46 +720,46 @@
         <v>47</v>
       </c>
       <c r="P1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" t="s">
         <v>55</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>56</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>57</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>58</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>59</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
+        <v>67</v>
+      </c>
+      <c r="W1" t="s">
+        <v>53</v>
+      </c>
+      <c r="X1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC1" t="s">
         <v>60</v>
-      </c>
-      <c r="V1" t="s">
-        <v>48</v>
-      </c>
-      <c r="W1" t="s">
-        <v>54</v>
-      </c>
-      <c r="X1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:29">
@@ -781,27 +785,27 @@
         <f>F2-C2</f>
         <v>75</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>9.1576768805289477E-2</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="3">
         <v>0.18315353761057895</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="3">
         <v>0.36630707522115791</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="3">
         <v>1.4652283008846316</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="3">
         <f>K2-H2</f>
         <v>1.3736515320793421</v>
       </c>
       <c r="M2">
         <v>54.598999999999997</v>
       </c>
-      <c r="N2">
-        <v>6652</v>
+      <c r="N2" s="3">
+        <v>15658</v>
       </c>
       <c r="O2">
         <v>5.42</v>
@@ -829,7 +833,7 @@
         <v>4.2616999447557404</v>
       </c>
       <c r="AC2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:29">
@@ -855,27 +859,27 @@
         <f t="shared" ref="G3:G35" si="0">F3-C3</f>
         <v>1474</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>0.4337107377647918</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="3">
         <v>5.0675675675675675</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="3">
         <v>10.614499634769905</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="3">
         <v>34.080533235938638</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="3">
         <f t="shared" ref="L3:L35" si="1">K3-H3</f>
         <v>33.646822498173847</v>
       </c>
       <c r="M3">
         <v>43.808</v>
       </c>
-      <c r="N3">
-        <v>5764</v>
+      <c r="N3" s="3">
+        <v>97105</v>
       </c>
       <c r="O3">
         <v>1.21</v>
@@ -903,7 +907,7 @@
         <v>36.839935525971505</v>
       </c>
       <c r="AC3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:29">
@@ -929,27 +933,27 @@
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>0.13178703215603585</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <v>0.65893516078017922</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="3">
         <v>3.0311017395888245</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="3">
         <v>10.015814443858725</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="3">
         <f t="shared" si="1"/>
         <v>9.8840274117026894</v>
       </c>
       <c r="M4">
         <v>15.176</v>
       </c>
-      <c r="N4">
-        <v>12240</v>
+      <c r="N4" s="3">
+        <v>18803</v>
       </c>
       <c r="O4">
         <v>3.41</v>
@@ -977,7 +981,7 @@
         <v>22.139529188778276</v>
       </c>
       <c r="AC4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:29">
@@ -1003,27 +1007,27 @@
         <f t="shared" si="0"/>
         <v>1311</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
         <v>1.0789863607005814</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="3">
         <v>3.069792181148133</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="3">
         <v>6.5423046236845108</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="3">
         <v>11.04061395843623</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="3">
         <f t="shared" si="1"/>
         <v>9.9616275977356494</v>
       </c>
       <c r="M5">
         <v>131.60499999999999</v>
       </c>
-      <c r="N5">
-        <v>4090</v>
+      <c r="N5" s="3">
+        <v>67736</v>
       </c>
       <c r="O5">
         <v>8.01</v>
@@ -1051,7 +1055,7 @@
         <v>22.727669796898887</v>
       </c>
       <c r="AC5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:29">
@@ -1077,27 +1081,27 @@
         <f t="shared" si="0"/>
         <v>124</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <v>4.9509852460639665E-2</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="3">
         <v>0.59411822952767601</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="3">
         <v>4.50539657391821</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="3">
         <v>6.188731557579958</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="3">
         <f t="shared" si="1"/>
         <v>6.1392217051193185</v>
       </c>
       <c r="M6">
         <v>20.198</v>
       </c>
-      <c r="N6">
-        <v>3536</v>
+      <c r="N6" s="3">
+        <v>7603</v>
       </c>
       <c r="O6">
         <v>3.22</v>
@@ -1125,7 +1129,7 @@
         <v>26.099888317167899</v>
       </c>
       <c r="AC6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:29">
@@ -1151,27 +1155,27 @@
         <f t="shared" si="0"/>
         <v>249</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <v>0</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="3">
         <v>1.2299114463758609</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="3">
         <v>7.7074450639553955</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="3">
         <v>20.416530009839292</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="3">
         <f t="shared" si="1"/>
         <v>20.416530009839292</v>
       </c>
       <c r="M7">
         <v>12.196</v>
       </c>
-      <c r="N7">
-        <v>6976</v>
+      <c r="N7" s="3">
+        <v>10201</v>
       </c>
       <c r="O7">
         <v>3.59</v>
@@ -1199,7 +1203,7 @@
         <v>19.942700101220915</v>
       </c>
       <c r="AC7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:29">
@@ -1225,27 +1229,27 @@
         <f t="shared" si="0"/>
         <v>237</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
         <v>0.20370747606437156</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="3">
         <v>3.7685883071908739</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="3">
         <v>17.111427989407211</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="3">
         <v>24.343043389692404</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="3">
         <f t="shared" si="1"/>
         <v>24.139335913628031</v>
       </c>
       <c r="M8">
         <v>9.8179999999999996</v>
       </c>
-      <c r="N8">
-        <v>2772</v>
+      <c r="N8" s="3">
+        <v>7848</v>
       </c>
       <c r="O8">
         <v>6.2</v>
@@ -1273,7 +1277,7 @@
         <v>10.197803791400467</v>
       </c>
       <c r="AC8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:29">
@@ -1299,27 +1303,27 @@
         <f t="shared" si="0"/>
         <v>10677</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="3">
         <v>7.0173790511977456</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="3">
         <v>39.220291216533582</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="3">
         <v>69.027712541099106</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="3">
         <v>107.3179896665101</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="3">
         <f t="shared" si="1"/>
         <v>100.30061061531235</v>
       </c>
       <c r="M9">
         <v>106.45</v>
       </c>
-      <c r="N9">
-        <v>1720</v>
+      <c r="N9" s="3">
+        <v>320114</v>
       </c>
       <c r="O9">
         <v>4.93</v>
@@ -1347,7 +1351,7 @@
         <v>24.466750853642896</v>
       </c>
       <c r="AC9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:29">
@@ -1373,27 +1377,27 @@
         <f t="shared" si="0"/>
         <v>115</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="3">
         <v>5.4378857500203916E-2</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="3">
         <v>0.87006172000326265</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="3">
         <v>2.6373745887598901</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="3">
         <v>3.1811631637619291</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="3">
         <f t="shared" si="1"/>
         <v>3.1267843062617251</v>
       </c>
       <c r="M10">
         <v>36.779000000000003</v>
       </c>
-      <c r="N10">
-        <v>6316</v>
+      <c r="N10" s="3">
+        <v>16900</v>
       </c>
       <c r="O10">
         <v>4.41</v>
@@ -1421,7 +1425,7 @@
         <v>14.419841381021262</v>
       </c>
       <c r="AC10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:29">
@@ -1447,27 +1451,27 @@
         <f t="shared" si="0"/>
         <v>3020</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="3">
         <v>0.39650991174650596</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="3">
         <v>2.0266062155932527</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="3">
         <v>4.5258202047833516</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="3">
         <v>6.4442873535366481</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="3">
         <f t="shared" si="1"/>
         <v>6.0477774417901422</v>
       </c>
       <c r="M11">
         <v>499.35700000000003</v>
       </c>
-      <c r="N11">
-        <v>31177</v>
+      <c r="N11" s="3">
+        <v>342772</v>
       </c>
       <c r="O11">
         <v>7.69</v>
@@ -1495,7 +1499,7 @@
         <v>23.118221912409346</v>
       </c>
       <c r="AC11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:29">
@@ -1521,27 +1525,27 @@
         <f t="shared" si="0"/>
         <v>3740</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="3">
         <v>0.26616981634282671</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="3">
         <v>2.0721177100237265</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="3">
         <v>4.0154435734299554</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="3">
         <v>10.970203290774784</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="3">
         <f t="shared" si="1"/>
         <v>10.704033474431958</v>
       </c>
       <c r="M12">
         <v>349.40100000000001</v>
       </c>
-      <c r="N12">
-        <v>31078</v>
+      <c r="N12" s="3">
+        <v>263980</v>
       </c>
       <c r="O12">
         <v>4.25</v>
@@ -1569,7 +1573,7 @@
         <v>21.477190311767259</v>
       </c>
       <c r="AC12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:29">
@@ -1595,27 +1599,27 @@
         <f t="shared" si="0"/>
         <v>12043</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="3">
         <v>0.2331627651599672</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="3">
         <v>2.401827193798372</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="3">
         <v>12.17711344496732</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="3">
         <v>30.426487290122171</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="3">
         <f t="shared" si="1"/>
         <v>30.193324524962204</v>
       </c>
       <c r="M13">
         <v>398.863</v>
       </c>
-      <c r="N13">
-        <v>15869</v>
+      <c r="N13" s="3">
+        <v>161217</v>
       </c>
       <c r="O13">
         <v>3.69</v>
@@ -1643,7 +1647,7 @@
         <v>27.155280620101067</v>
       </c>
       <c r="AC13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:29">
@@ -1669,27 +1673,27 @@
         <f t="shared" si="0"/>
         <v>312</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="3">
         <v>0.1752745968684272</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="3">
         <v>1.1295474020409753</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="3">
         <v>3.6807665342369713</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="3">
         <v>6.2514606216405699</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="3">
         <f t="shared" si="1"/>
         <v>6.0761860247721424</v>
       </c>
       <c r="M14">
         <v>51.347999999999999</v>
       </c>
-      <c r="N14">
-        <v>2618</v>
+      <c r="N14" s="3">
+        <v>18645</v>
       </c>
       <c r="O14">
         <v>4.5599999999999996</v>
@@ -1717,7 +1721,7 @@
         <v>21.512235056017239</v>
       </c>
       <c r="AC14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:29">
@@ -1743,27 +1747,27 @@
         <f t="shared" si="0"/>
         <v>3140</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="3">
         <v>0.18587360594795541</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="3">
         <v>3.949814126394052</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="3">
         <v>21.352230483271377</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="3">
         <v>73.141263940520446</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="3">
         <f t="shared" si="1"/>
         <v>72.955390334572485</v>
       </c>
       <c r="M15">
         <v>43.04</v>
       </c>
-      <c r="N15">
-        <v>13739</v>
+      <c r="N15" s="3">
+        <v>27994</v>
       </c>
       <c r="O15">
         <v>3.8</v>
@@ -1791,7 +1795,7 @@
         <v>17.457597543717412</v>
       </c>
       <c r="AC15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:29">
@@ -1817,27 +1821,27 @@
         <f t="shared" si="0"/>
         <v>885</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="3">
         <v>0.32500361115123499</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="3">
         <v>5.2361692907698973</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="3">
         <v>14.805720063556262</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="3">
         <v>32.283692041022675</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="3">
         <f t="shared" si="1"/>
         <v>31.95868842987144</v>
       </c>
       <c r="M16">
         <v>27.692</v>
       </c>
-      <c r="N16">
-        <v>1566</v>
+      <c r="N16" s="3">
+        <v>12371</v>
       </c>
       <c r="O16">
         <v>3.39</v>
@@ -1865,7 +1869,7 @@
         <v>20.110307223241186</v>
       </c>
       <c r="AC16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:29">
@@ -1891,27 +1895,27 @@
         <f t="shared" si="0"/>
         <v>498</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="3">
         <v>0.52718981469278015</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="3">
         <v>3.5321717584416272</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="3">
         <v>7.7760497667185078</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="3">
         <v>13.654216200543006</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="3">
         <f t="shared" si="1"/>
         <v>13.127026385850225</v>
       </c>
       <c r="M17">
         <v>37.936999999999998</v>
       </c>
-      <c r="N17">
-        <v>703</v>
+      <c r="N17" s="3">
+        <v>46689</v>
       </c>
       <c r="O17">
         <v>6.88</v>
@@ -1939,7 +1943,7 @@
         <v>9.3578182768762694</v>
       </c>
       <c r="AC17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:29">
@@ -1965,27 +1969,27 @@
         <f t="shared" si="0"/>
         <v>204</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="3">
         <v>0.26041666666666669</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="3">
         <v>13.020833333333334</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="3">
         <v>21.484375</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="3">
         <v>26.822916666666668</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="3">
         <f t="shared" si="1"/>
         <v>26.5625</v>
       </c>
       <c r="M18">
         <v>7.68</v>
       </c>
-      <c r="N18">
-        <v>4303</v>
+      <c r="N18" s="3">
+        <v>8721</v>
       </c>
       <c r="O18">
         <v>5.65</v>
@@ -2013,7 +2017,7 @@
         <v>18.990631463894225</v>
       </c>
       <c r="AC18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:29">
@@ -2039,27 +2043,27 @@
         <f t="shared" si="0"/>
         <v>286</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="3">
         <v>0.31219338150031217</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="3">
         <v>3.9693158505039694</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="3">
         <v>8.7860137365087851</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="3">
         <v>13.067522968513067</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="3">
         <f t="shared" si="1"/>
         <v>12.755329587012755</v>
       </c>
       <c r="M19">
         <v>22.422000000000001</v>
       </c>
-      <c r="N19">
-        <v>12333</v>
+      <c r="N19" s="3">
+        <v>42102</v>
       </c>
       <c r="O19">
         <v>5.57</v>
@@ -2087,7 +2091,7 @@
         <v>25.729657985400483</v>
       </c>
       <c r="AC19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:29">
@@ -2113,27 +2117,27 @@
         <f t="shared" si="0"/>
         <v>182</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="3">
         <v>9.388349058818006E-2</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="3">
         <v>0.53983007088203538</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="3">
         <v>1.5608130310284936</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="3">
         <v>2.2297329014692764</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="3">
         <f t="shared" si="1"/>
         <v>2.1358494108810961</v>
       </c>
       <c r="M20">
         <v>85.212000000000003</v>
       </c>
-      <c r="N20">
-        <v>1208</v>
+      <c r="N20" s="3">
+        <v>27571</v>
       </c>
       <c r="O20">
         <v>4.28</v>
@@ -2161,7 +2165,7 @@
         <v>19.169037296401708</v>
       </c>
       <c r="AC20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:29">
@@ -2187,27 +2191,27 @@
         <f t="shared" si="0"/>
         <v>727</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="3">
         <v>7.8198310916484201E-2</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="3">
         <v>3.1279324366593682</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="3">
         <v>11.964341570222082</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="3">
         <v>56.928370347200499</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="3">
         <f t="shared" si="1"/>
         <v>56.850172036284015</v>
       </c>
       <c r="M21">
         <v>12.788</v>
       </c>
-      <c r="N21">
-        <v>4234</v>
+      <c r="N21" s="3">
+        <v>3567</v>
       </c>
       <c r="O21">
         <v>4.26</v>
@@ -2235,7 +2239,7 @@
         <v>24.54959190581863</v>
       </c>
       <c r="AC21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:29">
@@ -2261,27 +2265,27 @@
         <f t="shared" si="0"/>
         <v>741</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="3">
         <v>5.4588132539985811E-2</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="3">
         <v>1.2555270484196737</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="3">
         <v>12.173153556416835</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="3">
         <v>40.504394344669471</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="3">
         <f t="shared" si="1"/>
         <v>40.449806212129488</v>
       </c>
       <c r="M22">
         <v>18.318999999999999</v>
       </c>
-      <c r="N22">
-        <v>1741</v>
+      <c r="N22" s="3">
+        <v>14365</v>
       </c>
       <c r="O22" s="1">
         <v>7.02</v>
@@ -2309,7 +2313,7 @@
         <v>30.91276127891911</v>
       </c>
       <c r="AC22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:29">
@@ -2335,27 +2339,27 @@
         <f t="shared" si="0"/>
         <v>1230</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="3">
         <v>7.8039644139222722E-2</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="3">
         <v>4.487279538005307</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="3">
         <v>12.408303418136413</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="3">
         <v>24.07523021695021</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="3">
         <f t="shared" si="1"/>
         <v>23.997190572810986</v>
       </c>
       <c r="M23">
         <v>51.256</v>
       </c>
-      <c r="N23">
-        <v>4406</v>
+      <c r="N23" s="3">
+        <v>48448</v>
       </c>
       <c r="O23">
         <v>3.14</v>
@@ -2383,7 +2387,7 @@
         <v>23.404604941439494</v>
       </c>
       <c r="AC23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:29">
@@ -2409,27 +2413,27 @@
         <f t="shared" si="0"/>
         <v>113</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="3">
         <v>0</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="3">
         <v>5.4137943479987002E-2</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="3">
         <v>1.6602302667196016</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="3">
         <v>2.0391958710795106</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="3">
         <f t="shared" si="1"/>
         <v>2.0391958710795106</v>
       </c>
       <c r="M24">
         <v>55.414000000000001</v>
       </c>
-      <c r="N24">
-        <v>5252</v>
+      <c r="N24" s="3">
+        <v>22865</v>
       </c>
       <c r="O24">
         <v>2.8</v>
@@ -2457,7 +2461,7 @@
         <v>18.092186380863229</v>
       </c>
       <c r="AC24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:29">
@@ -2483,27 +2487,27 @@
         <f t="shared" si="0"/>
         <v>1740</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="3">
         <v>0.29108691855388019</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="3">
         <v>5.9672818303545441</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="3">
         <v>19.648367002386912</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="3">
         <v>50.940210746929033</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="3">
         <f t="shared" si="1"/>
         <v>50.649123828375153</v>
       </c>
       <c r="M25">
         <v>34.353999999999999</v>
       </c>
-      <c r="N25">
-        <v>417</v>
+      <c r="N25" s="3">
+        <v>4525</v>
       </c>
       <c r="O25">
         <v>3.62</v>
@@ -2531,7 +2535,7 @@
         <v>16.200950512469316</v>
       </c>
       <c r="AC25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:29">
@@ -2557,27 +2561,27 @@
         <f t="shared" si="0"/>
         <v>223</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="3">
         <v>4.2085770800892215E-2</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="3">
         <v>0.57517220094552701</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="3">
         <v>1.6413450612347964</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="3">
         <v>3.1704614003338802</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="3">
         <f t="shared" si="1"/>
         <v>3.1283756295329881</v>
       </c>
       <c r="M26">
         <v>71.283000000000001</v>
       </c>
-      <c r="N26">
-        <v>9621</v>
+      <c r="N26" s="3">
+        <v>156146</v>
       </c>
       <c r="O26">
         <v>5.07</v>
@@ -2605,7 +2609,7 @@
         <v>11.098976360008555</v>
       </c>
       <c r="AC26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:29">
@@ -2631,27 +2635,27 @@
         <f t="shared" si="0"/>
         <v>114</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="3">
         <v>7.1174377224199281E-2</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="3">
         <v>2.9893238434163698</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="3">
         <v>6.5480427046263339</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="3">
         <v>8.185053380782918</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="3">
         <f t="shared" si="1"/>
         <v>8.1138790035587185</v>
       </c>
       <c r="M27">
         <v>14.05</v>
       </c>
-      <c r="N27">
-        <v>4394</v>
+      <c r="N27" s="3">
+        <v>6115</v>
       </c>
       <c r="O27">
         <v>2.61</v>
@@ -2679,7 +2683,7 @@
         <v>11.574105622589343</v>
       </c>
       <c r="AC27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:29">
@@ -2705,27 +2709,27 @@
         <f t="shared" si="0"/>
         <v>5034</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="3">
         <v>0.56003584229390679</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="3">
         <v>5.4995519713261647</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="3">
         <v>17.260304659498207</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="3">
         <v>56.944444444444443</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="3">
         <f t="shared" si="1"/>
         <v>56.384408602150536</v>
       </c>
       <c r="M28">
         <v>89.28</v>
       </c>
-      <c r="N28">
-        <v>14596</v>
+      <c r="N28" s="3">
+        <v>41908</v>
       </c>
       <c r="O28">
         <v>6.07</v>
@@ -2753,7 +2757,7 @@
         <v>20.656283078784217</v>
       </c>
       <c r="AC28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:29">
@@ -2779,27 +2783,27 @@
         <f t="shared" si="0"/>
         <v>186</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="3">
         <v>9.6867936712948022E-2</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="3">
         <v>1.517597675169519</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="3">
         <v>4.1330319664191153</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="3">
         <v>6.1026800129157248</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="3">
         <f t="shared" si="1"/>
         <v>6.0058120762027771</v>
       </c>
       <c r="M29">
         <v>30.97</v>
       </c>
-      <c r="N29">
-        <v>12566</v>
+      <c r="N29" s="3">
+        <v>23348</v>
       </c>
       <c r="O29">
         <v>2.98</v>
@@ -2827,7 +2831,7 @@
         <v>12.530378584672992</v>
       </c>
       <c r="AC29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:29">
@@ -2853,27 +2857,27 @@
         <f t="shared" si="0"/>
         <v>360</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="3">
         <v>0.10886921178690666</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="3">
         <v>2.2499637102627377</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="3">
         <v>8.8546958920017413</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="3">
         <v>13.173174626215706</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="3">
         <f t="shared" si="1"/>
         <v>13.0643054144288</v>
       </c>
       <c r="M30">
         <v>27.556000000000001</v>
       </c>
-      <c r="N30">
-        <v>28777</v>
+      <c r="N30" s="3">
+        <v>34454</v>
       </c>
       <c r="O30">
         <v>3.17</v>
@@ -2901,7 +2905,7 @@
         <v>17.985745045746683</v>
       </c>
       <c r="AC30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:29">
@@ -2927,27 +2931,27 @@
         <f t="shared" si="0"/>
         <v>1107</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="3">
         <v>7.9088895919012969E-2</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="3">
         <v>1.7795001581777918</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="3">
         <v>13.405567858272699</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="3">
         <v>43.854792787092691</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="3">
         <f t="shared" si="1"/>
         <v>43.775703891173677</v>
       </c>
       <c r="M31">
         <v>25.288</v>
       </c>
-      <c r="N31">
-        <v>14260</v>
+      <c r="N31" s="3">
+        <v>29557</v>
       </c>
       <c r="O31">
         <v>5.57</v>
@@ -2975,7 +2979,7 @@
         <v>24.202092398443035</v>
       </c>
       <c r="AC31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:29">
@@ -3001,27 +3005,27 @@
         <f t="shared" si="0"/>
         <v>718</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="3">
         <v>0.14548628791736379</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="3">
         <v>2.6914963264712299</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="3">
         <v>10.311340656143159</v>
       </c>
-      <c r="K32">
+      <c r="K32" s="3">
         <v>13.202880628500765</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="3">
         <f t="shared" si="1"/>
         <v>13.0573943405834</v>
       </c>
       <c r="M32">
         <v>54.988</v>
       </c>
-      <c r="N32">
-        <v>17030</v>
+      <c r="N32" s="3">
+        <v>39411</v>
       </c>
       <c r="O32">
         <v>5.22</v>
@@ -3049,7 +3053,7 @@
         <v>29.476906416315135</v>
       </c>
       <c r="AC32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:29">
@@ -3075,27 +3079,27 @@
         <f t="shared" si="0"/>
         <v>2044</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="3">
         <v>5.8357357112011107E-2</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="3">
         <v>1.7507207133603333</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="3">
         <v>11.461384936798982</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="3">
         <v>23.914844944502153</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="3">
         <f t="shared" si="1"/>
         <v>23.856487587390141</v>
       </c>
       <c r="M33">
         <v>85.679000000000002</v>
       </c>
-      <c r="N33">
-        <v>6352</v>
+      <c r="N33" s="3">
+        <v>56867</v>
       </c>
       <c r="O33">
         <v>3.86</v>
@@ -3123,7 +3127,7 @@
         <v>14.182387804904323</v>
       </c>
       <c r="AC33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:29">
@@ -3149,27 +3153,27 @@
         <f t="shared" si="0"/>
         <v>1532</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="3">
         <v>0.1292209337912742</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="3">
         <v>0.79572890808310948</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="3">
         <v>2.781650627401639</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="3">
         <v>10.548508858435067</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="3">
         <f t="shared" si="1"/>
         <v>10.419287924643793</v>
       </c>
       <c r="M34">
         <v>147.035</v>
       </c>
-      <c r="N34">
-        <v>18806</v>
+      <c r="N34" s="3">
+        <v>108407</v>
       </c>
       <c r="O34">
         <v>4.7300000000000004</v>
@@ -3197,7 +3201,7 @@
         <v>25.194644712605459</v>
       </c>
       <c r="AC34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:29">
@@ -3223,27 +3227,27 @@
         <f t="shared" si="0"/>
         <v>290</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="3">
         <v>0.5924323210468021</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="3">
         <v>2.447003065193313</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="3">
         <v>6.0788707724802311</v>
       </c>
-      <c r="K35">
+      <c r="K35" s="3">
         <v>8.0622311516369169</v>
       </c>
-      <c r="L35">
+      <c r="L35" s="3">
         <f t="shared" si="1"/>
         <v>7.4697988305901148</v>
       </c>
       <c r="M35">
         <v>38.823</v>
       </c>
-      <c r="N35">
-        <v>252</v>
+      <c r="N35" s="3">
+        <v>34728</v>
       </c>
       <c r="O35">
         <v>3.38</v>
@@ -3271,7 +3275,7 @@
         <v>23.30805387064655</v>
       </c>
       <c r="AC35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new data updated expandr
</commit_message>
<xml_diff>
--- a/processed data/explore expandr.xlsx
+++ b/processed data/explore expandr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mygithub\data-indonesia-covid19\processed data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6AC04C-D676-4C50-9005-7A58E9EB390C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AA3C47-51A9-41D7-A39E-D919351F8335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{99997AC6-4747-4E3C-BD2F-4A87F19432B6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="65">
   <si>
     <t>ID</t>
   </si>
@@ -190,18 +190,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>loan_q1_yoy</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>loan_q2_yoy</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>loan_q2_qtq</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>gdp_q2_yoy</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -266,7 +254,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>TTTshare_gdp</t>
+    <t>THS_share_gdp</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -647,2635 +635,2931 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0873AAB-CC92-48FA-A2C1-49CCA02E734A}">
-  <dimension ref="A1:AC35"/>
+  <dimension ref="A1:Z35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2:L35"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
   <cols>
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.83203125" customWidth="1"/>
-    <col min="16" max="16" width="10.08203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.08203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.83203125" customWidth="1"/>
-    <col min="22" max="22" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" customWidth="1"/>
+    <col min="17" max="17" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.83203125" customWidth="1"/>
+    <col min="23" max="23" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>40</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>41</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>45</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>42</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>46</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>47</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
         <v>55</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
         <v>56</v>
       </c>
-      <c r="S1" t="s">
-        <v>57</v>
-      </c>
-      <c r="T1" t="s">
-        <v>58</v>
-      </c>
-      <c r="U1" t="s">
-        <v>59</v>
-      </c>
-      <c r="V1" t="s">
-        <v>67</v>
-      </c>
       <c r="W1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="X1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Y1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="Z1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA1" t="s">
         <v>49</v>
       </c>
-      <c r="AB1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>60</v>
-      </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:26">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>20</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>80</v>
       </c>
-      <c r="G2">
-        <f>F2-C2</f>
+      <c r="H2">
+        <f>G2-D2</f>
         <v>75</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>9.1576768805289477E-2</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>0.18315353761057895</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="3">
         <v>0.36630707522115791</v>
       </c>
-      <c r="K2" s="3">
+      <c r="L2" s="3">
         <v>1.4652283008846316</v>
       </c>
-      <c r="L2" s="3">
-        <f>K2-H2</f>
+      <c r="M2" s="3">
+        <f>L2-I2</f>
         <v>1.3736515320793421</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>54.598999999999997</v>
       </c>
-      <c r="N2" s="3">
+      <c r="O2" s="3">
         <v>15658</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>5.42</v>
       </c>
-      <c r="P2" s="2">
+      <c r="Q2" s="2">
         <v>-16.197802197802197</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="R2" s="2">
         <v>-2.9450549450549453</v>
       </c>
-      <c r="R2" s="2">
+      <c r="S2" s="2">
         <v>-16.703296703296704</v>
       </c>
-      <c r="S2" s="2">
+      <c r="T2" s="2">
         <v>-43.219780219780219</v>
       </c>
-      <c r="T2" s="2">
+      <c r="U2" s="2">
         <v>-18.736263736263737</v>
       </c>
-      <c r="U2" s="2">
-        <f>AVERAGE(P2:T2)</f>
+      <c r="V2" s="2">
+        <f>AVERAGE(Q2:U2)</f>
         <v>-19.560439560439562</v>
       </c>
-      <c r="V2">
-        <v>4.2616999447557404</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>61</v>
+      <c r="W2">
+        <v>2.2886907110725279</v>
+      </c>
+      <c r="X2">
+        <v>3.17</v>
+      </c>
+      <c r="Y2">
+        <v>-1.82</v>
+      </c>
+      <c r="Z2">
+        <v>-1.28</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:26">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3">
         <v>19</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>222</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>465</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>1493</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G35" si="0">F3-C3</f>
+      <c r="H3">
+        <f t="shared" ref="H3:H35" si="0">G3-D3</f>
         <v>1474</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>0.4337107377647918</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J3" s="3">
         <v>5.0675675675675675</v>
       </c>
-      <c r="J3" s="3">
+      <c r="K3" s="3">
         <v>10.614499634769905</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="3">
         <v>34.080533235938638</v>
       </c>
-      <c r="L3" s="3">
-        <f t="shared" ref="L3:L35" si="1">K3-H3</f>
+      <c r="M3" s="3">
+        <f t="shared" ref="M3:M35" si="1">L3-I3</f>
         <v>33.646822498173847</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>43.808</v>
       </c>
-      <c r="N3" s="3">
+      <c r="O3" s="3">
         <v>97105</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>1.21</v>
       </c>
-      <c r="P3" s="2">
+      <c r="Q3" s="2">
         <v>-44</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="R3" s="2">
         <v>-33.560439560439562</v>
       </c>
-      <c r="R3" s="2">
+      <c r="S3" s="2">
         <v>-59.516483516483518</v>
       </c>
-      <c r="S3" s="2">
+      <c r="T3" s="2">
         <v>-75.307692307692307</v>
       </c>
-      <c r="T3" s="2">
+      <c r="U3" s="2">
         <v>-38.857142857142854</v>
       </c>
-      <c r="U3" s="2">
-        <f t="shared" ref="U3:U35" si="2">AVERAGE(P3:T3)</f>
+      <c r="V3" s="2">
+        <f t="shared" ref="V3:V35" si="2">AVERAGE(Q3:U3)</f>
         <v>-50.248351648351658</v>
       </c>
-      <c r="V3">
-        <v>36.839935525971505</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>62</v>
+      <c r="W3">
+        <v>30.219639496708801</v>
+      </c>
+      <c r="X3">
+        <v>-1.1399999999999999</v>
+      </c>
+      <c r="Y3">
+        <v>-10.98</v>
+      </c>
+      <c r="Z3">
+        <v>-7.22</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:26">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>46</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>152</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>0.13178703215603585</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>0.65893516078017922</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <v>3.0311017395888245</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>10.015814443858725</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <f t="shared" si="1"/>
         <v>9.8840274117026894</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>15.176</v>
       </c>
-      <c r="N4" s="3">
+      <c r="O4" s="3">
         <v>18803</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>3.41</v>
       </c>
-      <c r="P4" s="2">
+      <c r="Q4" s="2">
         <v>-30.340659340659339</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="R4" s="2">
         <v>-7.813186813186813</v>
       </c>
-      <c r="R4" s="2">
+      <c r="S4" s="2">
         <v>-24.64835164835165</v>
       </c>
-      <c r="S4" s="2">
+      <c r="T4" s="2">
         <v>-63.989010989010985</v>
       </c>
-      <c r="T4" s="2">
+      <c r="U4" s="2">
         <v>-22.285714285714285</v>
       </c>
-      <c r="U4" s="2">
+      <c r="V4" s="2">
         <f t="shared" si="2"/>
         <v>-29.815384615384612</v>
       </c>
-      <c r="V4">
-        <v>22.139529188778276</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>61</v>
+      <c r="W4">
+        <v>8.1665409904746689</v>
+      </c>
+      <c r="X4">
+        <v>1.35</v>
+      </c>
+      <c r="Y4">
+        <v>-4.9800000000000004</v>
+      </c>
+      <c r="Z4">
+        <v>-2.38</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:26">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5">
         <v>142</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>404</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>861</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>1453</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <f t="shared" si="0"/>
         <v>1311</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>1.0789863607005814</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="3">
         <v>3.069792181148133</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <v>6.5423046236845108</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <v>11.04061395843623</v>
       </c>
-      <c r="L5" s="3">
+      <c r="M5" s="3">
         <f t="shared" si="1"/>
         <v>9.9616275977356494</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>131.60499999999999</v>
       </c>
-      <c r="N5" s="3">
+      <c r="O5" s="3">
         <v>67736</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>8.01</v>
       </c>
-      <c r="P5" s="2">
+      <c r="Q5" s="2">
         <v>-31.032967032967033</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="R5" s="2">
         <v>-12.428571428571429</v>
       </c>
-      <c r="R5" s="2">
+      <c r="S5" s="2">
         <v>-20.285714285714285</v>
       </c>
-      <c r="S5" s="2">
+      <c r="T5" s="2">
         <v>-61.989010989010985</v>
       </c>
-      <c r="T5" s="2">
+      <c r="U5" s="2">
         <v>-31.901098901098901</v>
       </c>
-      <c r="U5" s="2">
+      <c r="V5" s="2">
         <f t="shared" si="2"/>
         <v>-31.527472527472526</v>
       </c>
-      <c r="V5">
-        <v>22.727669796898887</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>62</v>
+      <c r="W5">
+        <v>11.572395719589428</v>
+      </c>
+      <c r="X5">
+        <v>3.19</v>
+      </c>
+      <c r="Y5">
+        <v>-7.4</v>
+      </c>
+      <c r="Z5">
+        <v>-8.5500000000000007</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:26">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>12</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>91</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>125</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <f t="shared" si="0"/>
         <v>124</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <v>4.9509852460639665E-2</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J6" s="3">
         <v>0.59411822952767601</v>
       </c>
-      <c r="J6" s="3">
+      <c r="K6" s="3">
         <v>4.50539657391821</v>
       </c>
-      <c r="K6" s="3">
+      <c r="L6" s="3">
         <v>6.188731557579958</v>
       </c>
-      <c r="L6" s="3">
+      <c r="M6" s="3">
         <f t="shared" si="1"/>
         <v>6.1392217051193185</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>20.198</v>
       </c>
-      <c r="N6" s="3">
+      <c r="O6" s="3">
         <v>7603</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>3.22</v>
       </c>
-      <c r="P6" s="2">
+      <c r="Q6" s="2">
         <v>-22.065934065934066</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="R6" s="2">
         <v>-9.4065934065934069</v>
       </c>
-      <c r="R6" s="2">
+      <c r="S6" s="2">
         <v>-27.164835164835164</v>
       </c>
-      <c r="S6" s="2">
+      <c r="T6" s="2">
         <v>-52.879120879120876</v>
       </c>
-      <c r="T6" s="2">
+      <c r="U6" s="2">
         <v>-23.35164835164835</v>
       </c>
-      <c r="U6" s="2">
+      <c r="V6" s="2">
         <f t="shared" si="2"/>
         <v>-26.97362637362637</v>
       </c>
-      <c r="V6">
-        <v>26.099888317167899</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>61</v>
+      <c r="W6">
+        <v>13.031912697455718</v>
+      </c>
+      <c r="X6">
+        <v>3.8</v>
+      </c>
+      <c r="Y6">
+        <v>-0.48</v>
+      </c>
+      <c r="Z6">
+        <v>-2.98</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:26">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>15</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>94</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>249</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <f t="shared" si="0"/>
         <v>249</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="3">
         <v>0</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J7" s="3">
         <v>1.2299114463758609</v>
       </c>
-      <c r="J7" s="3">
+      <c r="K7" s="3">
         <v>7.7074450639553955</v>
       </c>
-      <c r="K7" s="3">
+      <c r="L7" s="3">
         <v>20.416530009839292</v>
       </c>
-      <c r="L7" s="3">
+      <c r="M7" s="3">
         <f t="shared" si="1"/>
         <v>20.416530009839292</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>12.196</v>
       </c>
-      <c r="N7" s="3">
+      <c r="O7" s="3">
         <v>10201</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>3.59</v>
       </c>
-      <c r="P7" s="2">
+      <c r="Q7" s="2">
         <v>-30.219780219780219</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="R7" s="2">
         <v>-16.912087912087912</v>
       </c>
-      <c r="R7" s="2">
+      <c r="S7" s="2">
         <v>-13.406593406593407</v>
       </c>
-      <c r="S7" s="2">
+      <c r="T7" s="2">
         <v>-45.684210526315788</v>
       </c>
-      <c r="T7" s="2">
+      <c r="U7" s="2">
         <v>-26.098901098901099</v>
       </c>
-      <c r="U7" s="2">
+      <c r="V7" s="2">
         <f t="shared" si="2"/>
         <v>-26.464314632735686</v>
       </c>
-      <c r="V7">
-        <v>19.942700101220915</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>63</v>
+      <c r="W7">
+        <v>9.7732342085882333</v>
+      </c>
+      <c r="X7">
+        <v>4.05</v>
+      </c>
+      <c r="Y7">
+        <v>-0.27</v>
+      </c>
+      <c r="Z7">
+        <v>-3.77</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:26">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>37</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>168</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>239</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <f t="shared" si="0"/>
         <v>237</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <v>0.20370747606437156</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="3">
         <v>3.7685883071908739</v>
       </c>
-      <c r="J8" s="3">
+      <c r="K8" s="3">
         <v>17.111427989407211</v>
       </c>
-      <c r="K8" s="3">
+      <c r="L8" s="3">
         <v>24.343043389692404</v>
       </c>
-      <c r="L8" s="3">
+      <c r="M8" s="3">
         <f t="shared" si="1"/>
         <v>24.139335913628031</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>9.8179999999999996</v>
       </c>
-      <c r="N8" s="3">
+      <c r="O8" s="3">
         <v>7848</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>6.2</v>
       </c>
-      <c r="P8" s="2">
+      <c r="Q8" s="2">
         <v>-30.582417582417584</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="R8" s="2">
         <v>-16.318681318681318</v>
       </c>
-      <c r="R8" s="2">
+      <c r="S8" s="2">
         <v>-34.934065934065934</v>
       </c>
-      <c r="S8" s="2">
+      <c r="T8" s="2">
         <v>-61.912087912087912</v>
       </c>
-      <c r="T8" s="2">
+      <c r="U8" s="2">
         <v>-23.87912087912088</v>
       </c>
-      <c r="U8" s="2">
+      <c r="V8" s="2">
         <f t="shared" si="2"/>
         <v>-33.525274725274727</v>
       </c>
-      <c r="V8">
-        <v>10.197803791400467</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>64</v>
+      <c r="W8">
+        <v>3.6873746203362798</v>
+      </c>
+      <c r="X8">
+        <v>5.14</v>
+      </c>
+      <c r="Y8">
+        <v>0.53</v>
+      </c>
+      <c r="Z8">
+        <v>-2.75</v>
       </c>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:26">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9">
         <v>747</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>4175</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>7348</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>11424</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <f t="shared" si="0"/>
         <v>10677</v>
       </c>
-      <c r="H9" s="3">
+      <c r="I9" s="3">
         <v>7.0173790511977456</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J9" s="3">
         <v>39.220291216533582</v>
       </c>
-      <c r="J9" s="3">
+      <c r="K9" s="3">
         <v>69.027712541099106</v>
       </c>
-      <c r="K9" s="3">
+      <c r="L9" s="3">
         <v>107.3179896665101</v>
       </c>
-      <c r="L9" s="3">
+      <c r="M9" s="3">
         <f t="shared" si="1"/>
         <v>100.30061061531235</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>106.45</v>
       </c>
-      <c r="N9" s="3">
+      <c r="O9" s="3">
         <v>320114</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>4.93</v>
       </c>
-      <c r="P9" s="2">
+      <c r="Q9" s="2">
         <v>-27</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="R9" s="2">
         <v>-3</v>
       </c>
-      <c r="R9" s="2">
+      <c r="S9" s="2">
         <v>-77</v>
       </c>
-      <c r="S9" s="2">
+      <c r="T9" s="2">
         <v>-45</v>
       </c>
-      <c r="T9" s="2">
+      <c r="U9" s="2">
         <v>-33</v>
       </c>
-      <c r="U9" s="2">
+      <c r="V9" s="2">
         <f t="shared" si="2"/>
         <v>-37</v>
       </c>
-      <c r="V9">
-        <v>24.466750853642896</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>62</v>
+      <c r="W9">
+        <v>20.972147115654213</v>
+      </c>
+      <c r="X9">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="Y9">
+        <v>-8.2200000000000006</v>
+      </c>
+      <c r="Z9">
+        <v>-11.38</v>
       </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:26">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10">
         <v>2</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>32</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>97</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>117</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <f t="shared" si="0"/>
         <v>115</v>
       </c>
-      <c r="H10" s="3">
+      <c r="I10" s="3">
         <v>5.4378857500203916E-2</v>
       </c>
-      <c r="I10" s="3">
+      <c r="J10" s="3">
         <v>0.87006172000326265</v>
       </c>
-      <c r="J10" s="3">
+      <c r="K10" s="3">
         <v>2.6373745887598901</v>
       </c>
-      <c r="K10" s="3">
+      <c r="L10" s="3">
         <v>3.1811631637619291</v>
       </c>
-      <c r="L10" s="3">
+      <c r="M10" s="3">
         <f t="shared" si="1"/>
         <v>3.1267843062617251</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>36.779000000000003</v>
       </c>
-      <c r="N10" s="3">
+      <c r="O10" s="3">
         <v>16900</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>4.41</v>
       </c>
-      <c r="P10" s="2">
+      <c r="Q10" s="2">
         <v>-10</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="R10" s="2">
         <v>3</v>
       </c>
-      <c r="R10" s="2">
+      <c r="S10" s="2">
         <v>-7</v>
       </c>
-      <c r="S10" s="2">
+      <c r="T10" s="2">
         <v>-27</v>
       </c>
-      <c r="T10" s="2">
+      <c r="U10" s="2">
         <v>-17</v>
       </c>
-      <c r="U10" s="2">
+      <c r="V10" s="2">
         <f t="shared" si="2"/>
         <v>-11.6</v>
       </c>
-      <c r="V10">
-        <v>14.419841381021262</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>61</v>
+      <c r="W10">
+        <v>6.4869964822873962</v>
+      </c>
+      <c r="X10">
+        <v>1.87</v>
+      </c>
+      <c r="Y10">
+        <v>-1.72</v>
+      </c>
+      <c r="Z10">
+        <v>-1.41</v>
       </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:26">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11">
         <v>198</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1012</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>2260</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>3218</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <f t="shared" si="0"/>
         <v>3020</v>
       </c>
-      <c r="H11" s="3">
+      <c r="I11" s="3">
         <v>0.39650991174650596</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <v>2.0266062155932527</v>
       </c>
-      <c r="J11" s="3">
+      <c r="K11" s="3">
         <v>4.5258202047833516</v>
       </c>
-      <c r="K11" s="3">
+      <c r="L11" s="3">
         <v>6.4442873535366481</v>
       </c>
-      <c r="L11" s="3">
+      <c r="M11" s="3">
         <f t="shared" si="1"/>
         <v>6.0477774417901422</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>499.35700000000003</v>
       </c>
-      <c r="N11" s="3">
+      <c r="O11" s="3">
         <v>342772</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>7.69</v>
       </c>
-      <c r="P11" s="2">
+      <c r="Q11" s="2">
         <v>-23</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="R11" s="2">
         <v>9</v>
       </c>
-      <c r="R11" s="2">
+      <c r="S11" s="2">
         <v>-2</v>
       </c>
-      <c r="S11" s="2">
+      <c r="T11" s="2">
         <v>-29</v>
       </c>
-      <c r="T11" s="2">
+      <c r="U11" s="2">
         <v>-25</v>
       </c>
-      <c r="U11" s="2">
+      <c r="V11" s="2">
         <f t="shared" si="2"/>
         <v>-14</v>
       </c>
-      <c r="V11">
-        <v>23.118221912409346</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>62</v>
+      <c r="W11">
+        <v>10.171990830730458</v>
+      </c>
+      <c r="X11">
+        <v>2.73</v>
+      </c>
+      <c r="Y11">
+        <v>-5.98</v>
+      </c>
+      <c r="Z11">
+        <v>-4.95</v>
       </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:26">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12">
         <v>93</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>724</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>1403</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>3833</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <f t="shared" si="0"/>
         <v>3740</v>
       </c>
-      <c r="H12" s="3">
+      <c r="I12" s="3">
         <v>0.26616981634282671</v>
       </c>
-      <c r="I12" s="3">
+      <c r="J12" s="3">
         <v>2.0721177100237265</v>
       </c>
-      <c r="J12" s="3">
+      <c r="K12" s="3">
         <v>4.0154435734299554</v>
       </c>
-      <c r="K12" s="3">
+      <c r="L12" s="3">
         <v>10.970203290774784</v>
       </c>
-      <c r="L12" s="3">
+      <c r="M12" s="3">
         <f t="shared" si="1"/>
         <v>10.704033474431958</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>349.40100000000001</v>
       </c>
-      <c r="N12" s="3">
+      <c r="O12" s="3">
         <v>263980</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>4.25</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>-6</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>2</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>-9</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>-34</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>-20</v>
       </c>
-      <c r="U12" s="2">
+      <c r="V12" s="2">
         <f t="shared" si="2"/>
         <v>-13.4</v>
       </c>
-      <c r="V12">
-        <v>21.477190311767259</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>62</v>
+      <c r="W12">
+        <v>9.0397164957138862</v>
+      </c>
+      <c r="X12">
+        <v>2.61</v>
+      </c>
+      <c r="Y12">
+        <v>-5.94</v>
+      </c>
+      <c r="Z12">
+        <v>-5.17</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:26">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13">
         <v>93</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>958</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>4857</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>12136</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <f t="shared" si="0"/>
         <v>12043</v>
       </c>
-      <c r="H13" s="3">
+      <c r="I13" s="3">
         <v>0.2331627651599672</v>
       </c>
-      <c r="I13" s="3">
+      <c r="J13" s="3">
         <v>2.401827193798372</v>
       </c>
-      <c r="J13" s="3">
+      <c r="K13" s="3">
         <v>12.17711344496732</v>
       </c>
-      <c r="K13" s="3">
+      <c r="L13" s="3">
         <v>30.426487290122171</v>
       </c>
-      <c r="L13" s="3">
+      <c r="M13" s="3">
         <f t="shared" si="1"/>
         <v>30.193324524962204</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>398.863</v>
       </c>
-      <c r="N13" s="3">
+      <c r="O13" s="3">
         <v>161217</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>3.69</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>-11</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>-1</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>-14</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>-37</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>-23</v>
       </c>
-      <c r="U13" s="2">
+      <c r="V13" s="2">
         <f t="shared" si="2"/>
         <v>-17.2</v>
       </c>
-      <c r="V13">
-        <v>27.155280620101067</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>62</v>
+      <c r="W13">
+        <v>10.726832364448653</v>
+      </c>
+      <c r="X13">
+        <v>3.02</v>
+      </c>
+      <c r="Y13">
+        <v>-5.9</v>
+      </c>
+      <c r="Z13">
+        <v>-5.45</v>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:26">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14">
         <v>9</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>58</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>189</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>321</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <f t="shared" si="0"/>
         <v>312</v>
       </c>
-      <c r="H14" s="3">
+      <c r="I14" s="3">
         <v>0.1752745968684272</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J14" s="3">
         <v>1.1295474020409753</v>
       </c>
-      <c r="J14" s="3">
+      <c r="K14" s="3">
         <v>3.6807665342369713</v>
       </c>
-      <c r="K14" s="3">
+      <c r="L14" s="3">
         <v>6.2514606216405699</v>
       </c>
-      <c r="L14" s="3">
+      <c r="M14" s="3">
         <f t="shared" si="1"/>
         <v>6.0761860247721424</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>51.347999999999999</v>
       </c>
-      <c r="N14" s="3">
+      <c r="O14" s="3">
         <v>18645</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>4.5599999999999996</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>-19</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>-6</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>-11</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>-36</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>-20</v>
       </c>
-      <c r="U14" s="2">
+      <c r="V14" s="2">
         <f t="shared" si="2"/>
         <v>-18.399999999999999</v>
       </c>
-      <c r="V14">
-        <v>21.512235056017239</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>65</v>
+      <c r="W14">
+        <v>8.1691805691351131</v>
+      </c>
+      <c r="X14">
+        <v>2.69</v>
+      </c>
+      <c r="Y14">
+        <v>-3.4</v>
+      </c>
+      <c r="Z14">
+        <v>-8.26</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:26">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15">
         <v>8</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>170</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>919</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>3148</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f t="shared" si="0"/>
         <v>3140</v>
       </c>
-      <c r="H15" s="3">
+      <c r="I15" s="3">
         <v>0.18587360594795541</v>
       </c>
-      <c r="I15" s="3">
+      <c r="J15" s="3">
         <v>3.949814126394052</v>
       </c>
-      <c r="J15" s="3">
+      <c r="K15" s="3">
         <v>21.352230483271377</v>
       </c>
-      <c r="K15" s="3">
+      <c r="L15" s="3">
         <v>73.141263940520446</v>
       </c>
-      <c r="L15" s="3">
+      <c r="M15" s="3">
         <f t="shared" si="1"/>
         <v>72.955390334572485</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>43.04</v>
       </c>
-      <c r="N15" s="3">
+      <c r="O15" s="3">
         <v>27994</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>3.8</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>-16</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>-8</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>-19</v>
       </c>
-      <c r="S15">
+      <c r="T15">
         <v>-38</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>-23</v>
       </c>
-      <c r="U15" s="2">
+      <c r="V15" s="2">
         <f t="shared" si="2"/>
         <v>-20.8</v>
       </c>
-      <c r="V15">
-        <v>17.457597543717412</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>65</v>
+      <c r="W15">
+        <v>9.9414362909659104</v>
+      </c>
+      <c r="X15">
+        <v>4.18</v>
+      </c>
+      <c r="Y15">
+        <v>-2.61</v>
+      </c>
+      <c r="Z15">
+        <v>-0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:26">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16">
         <v>9</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>145</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>410</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>894</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <f t="shared" si="0"/>
         <v>885</v>
       </c>
-      <c r="H16" s="3">
+      <c r="I16" s="3">
         <v>0.32500361115123499</v>
       </c>
-      <c r="I16" s="3">
+      <c r="J16" s="3">
         <v>5.2361692907698973</v>
       </c>
-      <c r="J16" s="3">
+      <c r="K16" s="3">
         <v>14.805720063556262</v>
       </c>
-      <c r="K16" s="3">
+      <c r="L16" s="3">
         <v>32.283692041022675</v>
       </c>
-      <c r="L16" s="3">
+      <c r="M16" s="3">
         <f t="shared" si="1"/>
         <v>31.95868842987144</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>27.692</v>
       </c>
-      <c r="N16" s="3">
+      <c r="O16" s="3">
         <v>12371</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>3.39</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>-17</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>-9</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>-20</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>-23</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>-17</v>
       </c>
-      <c r="U16" s="2">
+      <c r="V16" s="2">
         <f t="shared" si="2"/>
         <v>-17.2</v>
       </c>
-      <c r="V16">
-        <v>20.110307223241186</v>
-      </c>
-      <c r="AC16" t="s">
-        <v>65</v>
+      <c r="W16">
+        <v>9.2255592530414638</v>
+      </c>
+      <c r="X16">
+        <v>2.95</v>
+      </c>
+      <c r="Y16">
+        <v>-3.15</v>
+      </c>
+      <c r="Z16">
+        <v>-5.62</v>
       </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:26">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17">
         <v>20</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>134</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>295</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>518</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <f t="shared" si="0"/>
         <v>498</v>
       </c>
-      <c r="H17" s="3">
+      <c r="I17" s="3">
         <v>0.52718981469278015</v>
       </c>
-      <c r="I17" s="3">
+      <c r="J17" s="3">
         <v>3.5321717584416272</v>
       </c>
-      <c r="J17" s="3">
+      <c r="K17" s="3">
         <v>7.7760497667185078</v>
       </c>
-      <c r="K17" s="3">
+      <c r="L17" s="3">
         <v>13.654216200543006</v>
       </c>
-      <c r="L17" s="3">
+      <c r="M17" s="3">
         <f t="shared" si="1"/>
         <v>13.127026385850225</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>37.936999999999998</v>
       </c>
-      <c r="N17" s="3">
+      <c r="O17" s="3">
         <v>46689</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>6.88</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>-11</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>3</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <v>-5</v>
       </c>
-      <c r="S17">
+      <c r="T17">
         <v>-34</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>-17</v>
       </c>
-      <c r="U17" s="2">
+      <c r="V17" s="2">
         <f t="shared" si="2"/>
         <v>-12.8</v>
       </c>
-      <c r="V17">
-        <v>9.3578182768762694</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>65</v>
+      <c r="W17">
+        <v>4.5639687568988663</v>
+      </c>
+      <c r="X17">
+        <v>1.27</v>
+      </c>
+      <c r="Y17">
+        <v>-5.46</v>
+      </c>
+      <c r="Z17">
+        <v>-6.53</v>
       </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:26">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18">
         <v>2</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>100</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>165</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>206</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <f t="shared" si="0"/>
         <v>204</v>
       </c>
-      <c r="H18" s="3">
+      <c r="I18" s="3">
         <v>0.26041666666666669</v>
       </c>
-      <c r="I18" s="3">
+      <c r="J18" s="3">
         <v>13.020833333333334</v>
       </c>
-      <c r="J18" s="3">
+      <c r="K18" s="3">
         <v>21.484375</v>
       </c>
-      <c r="K18" s="3">
+      <c r="L18" s="3">
         <v>26.822916666666668</v>
       </c>
-      <c r="L18" s="3">
+      <c r="M18" s="3">
         <f t="shared" si="1"/>
         <v>26.5625</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>7.68</v>
       </c>
-      <c r="N18" s="3">
+      <c r="O18" s="3">
         <v>8721</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>5.65</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>-13</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <v>5</v>
       </c>
-      <c r="R18">
+      <c r="S18">
         <v>-10</v>
       </c>
-      <c r="S18">
+      <c r="T18">
         <v>-25</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <v>-12</v>
       </c>
-      <c r="U18" s="2">
+      <c r="V18" s="2">
         <f t="shared" si="2"/>
         <v>-11</v>
       </c>
-      <c r="V18">
-        <v>18.990631463894225</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>65</v>
+      <c r="W18">
+        <v>8.7372333673388471</v>
+      </c>
+      <c r="X18">
+        <v>5.01</v>
+      </c>
+      <c r="Y18">
+        <v>-3.35</v>
+      </c>
+      <c r="Z18">
+        <v>-6.95</v>
       </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:26">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19">
         <v>7</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>89</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>197</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>293</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <f t="shared" si="0"/>
         <v>286</v>
       </c>
-      <c r="H19" s="3">
+      <c r="I19" s="3">
         <v>0.31219338150031217</v>
       </c>
-      <c r="I19" s="3">
+      <c r="J19" s="3">
         <v>3.9693158505039694</v>
       </c>
-      <c r="J19" s="3">
+      <c r="K19" s="3">
         <v>8.7860137365087851</v>
       </c>
-      <c r="K19" s="3">
+      <c r="L19" s="3">
         <v>13.067522968513067</v>
       </c>
-      <c r="L19" s="3">
+      <c r="M19" s="3">
         <f t="shared" si="1"/>
         <v>12.755329587012755</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>22.422000000000001</v>
       </c>
-      <c r="N19" s="3">
+      <c r="O19" s="3">
         <v>42102</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>5.57</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <v>-16</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>-7</v>
       </c>
-      <c r="R19">
+      <c r="S19">
         <v>-14</v>
       </c>
-      <c r="S19">
+      <c r="T19">
         <v>-57</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>-16</v>
       </c>
-      <c r="U19" s="2">
+      <c r="V19" s="2">
         <f t="shared" si="2"/>
         <v>-22</v>
       </c>
-      <c r="V19">
-        <v>25.729657985400483</v>
-      </c>
-      <c r="AC19" t="s">
-        <v>61</v>
+      <c r="W19">
+        <v>9.9853993028321035</v>
+      </c>
+      <c r="X19">
+        <v>2.06</v>
+      </c>
+      <c r="Y19">
+        <v>-6.66</v>
+      </c>
+      <c r="Z19">
+        <v>-7.55</v>
       </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:26">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20">
         <v>8</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>46</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>133</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>190</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <f t="shared" si="0"/>
         <v>182</v>
       </c>
-      <c r="H20" s="3">
+      <c r="I20" s="3">
         <v>9.388349058818006E-2</v>
       </c>
-      <c r="I20" s="3">
+      <c r="J20" s="3">
         <v>0.53983007088203538</v>
       </c>
-      <c r="J20" s="3">
+      <c r="K20" s="3">
         <v>1.5608130310284936</v>
       </c>
-      <c r="K20" s="3">
+      <c r="L20" s="3">
         <v>2.2297329014692764</v>
       </c>
-      <c r="L20" s="3">
+      <c r="M20" s="3">
         <f t="shared" si="1"/>
         <v>2.1358494108810961</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>85.212000000000003</v>
       </c>
-      <c r="N20" s="3">
+      <c r="O20" s="3">
         <v>27571</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <v>4.28</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <v>-6</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <v>8</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <v>-12</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <v>-30</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>-23</v>
       </c>
-      <c r="U20" s="2">
+      <c r="V20" s="2">
         <f t="shared" si="2"/>
         <v>-12.6</v>
       </c>
-      <c r="V20">
-        <v>19.169037296401708</v>
-      </c>
-      <c r="AC20" t="s">
-        <v>61</v>
+      <c r="W20">
+        <v>7.8565402319458526</v>
+      </c>
+      <c r="X20">
+        <v>1.74</v>
+      </c>
+      <c r="Y20">
+        <v>-3.57</v>
+      </c>
+      <c r="Z20">
+        <v>-0.56000000000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:26">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21">
         <v>1</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>40</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>153</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>728</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <f t="shared" si="0"/>
         <v>727</v>
       </c>
-      <c r="H21" s="3">
+      <c r="I21" s="3">
         <v>7.8198310916484201E-2</v>
       </c>
-      <c r="I21" s="3">
+      <c r="J21" s="3">
         <v>3.1279324366593682</v>
       </c>
-      <c r="J21" s="3">
+      <c r="K21" s="3">
         <v>11.964341570222082</v>
       </c>
-      <c r="K21" s="3">
+      <c r="L21" s="3">
         <v>56.928370347200499</v>
       </c>
-      <c r="L21" s="3">
+      <c r="M21" s="3">
         <f t="shared" si="1"/>
         <v>56.850172036284015</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>12.788</v>
       </c>
-      <c r="N21" s="3">
+      <c r="O21" s="3">
         <v>3567</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>4.26</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <v>-22</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <v>5</v>
       </c>
-      <c r="R21">
+      <c r="S21">
         <v>-20</v>
       </c>
-      <c r="S21">
+      <c r="T21">
         <v>-31</v>
       </c>
-      <c r="T21">
+      <c r="U21">
         <v>-15</v>
       </c>
-      <c r="U21" s="2">
+      <c r="V21" s="2">
         <f t="shared" si="2"/>
         <v>-16.600000000000001</v>
       </c>
-      <c r="V21">
-        <v>24.54959190581863</v>
-      </c>
-      <c r="AC21" t="s">
-        <v>64</v>
+      <c r="W21">
+        <v>7.4434874186632571</v>
+      </c>
+      <c r="X21">
+        <v>3.06</v>
+      </c>
+      <c r="Y21">
+        <v>-0.16</v>
+      </c>
+      <c r="Z21">
+        <v>-1.35</v>
       </c>
     </row>
-    <row r="22" spans="1:29">
+    <row r="22" spans="1:26">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22">
         <v>1</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>23</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>223</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>742</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <f t="shared" si="0"/>
         <v>741</v>
       </c>
-      <c r="H22" s="3">
+      <c r="I22" s="3">
         <v>5.4588132539985811E-2</v>
       </c>
-      <c r="I22" s="3">
+      <c r="J22" s="3">
         <v>1.2555270484196737</v>
       </c>
-      <c r="J22" s="3">
+      <c r="K22" s="3">
         <v>12.173153556416835</v>
       </c>
-      <c r="K22" s="3">
+      <c r="L22" s="3">
         <v>40.504394344669471</v>
       </c>
-      <c r="L22" s="3">
+      <c r="M22" s="3">
         <f t="shared" si="1"/>
         <v>40.449806212129488</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>18.318999999999999</v>
       </c>
-      <c r="N22" s="3">
+      <c r="O22" s="3">
         <v>14365</v>
       </c>
-      <c r="O22" s="1">
+      <c r="P22" s="1">
         <v>7.02</v>
       </c>
-      <c r="P22">
+      <c r="Q22">
         <v>-47</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <v>-38</v>
       </c>
-      <c r="R22">
+      <c r="S22">
         <v>-31</v>
       </c>
-      <c r="S22">
+      <c r="T22">
         <v>-57</v>
       </c>
-      <c r="T22">
+      <c r="U22">
         <v>-31</v>
       </c>
-      <c r="U22" s="2">
+      <c r="V22" s="2">
         <f t="shared" si="2"/>
         <v>-40.799999999999997</v>
       </c>
-      <c r="V22">
-        <v>30.91276127891911</v>
-      </c>
-      <c r="AC22" t="s">
-        <v>64</v>
+      <c r="W22">
+        <v>14.107633440849199</v>
+      </c>
+      <c r="X22">
+        <v>4</v>
+      </c>
+      <c r="Y22">
+        <v>-0.92</v>
+      </c>
+      <c r="Z22">
+        <v>-2.61</v>
       </c>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:26">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23">
         <v>4</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>230</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>636</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>1234</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <f t="shared" si="0"/>
         <v>1230</v>
       </c>
-      <c r="H23" s="3">
+      <c r="I23" s="3">
         <v>7.8039644139222722E-2</v>
       </c>
-      <c r="I23" s="3">
+      <c r="J23" s="3">
         <v>4.487279538005307</v>
       </c>
-      <c r="J23" s="3">
+      <c r="K23" s="3">
         <v>12.408303418136413</v>
       </c>
-      <c r="K23" s="3">
+      <c r="L23" s="3">
         <v>24.07523021695021</v>
       </c>
-      <c r="L23" s="3">
+      <c r="M23" s="3">
         <f t="shared" si="1"/>
         <v>23.997190572810986</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>51.256</v>
       </c>
-      <c r="N23" s="3">
+      <c r="O23" s="3">
         <v>48448</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>3.14</v>
       </c>
-      <c r="P23">
+      <c r="Q23">
         <v>-17</v>
       </c>
-      <c r="Q23">
+      <c r="R23">
         <v>-6</v>
       </c>
-      <c r="R23">
+      <c r="S23">
         <v>-18</v>
       </c>
-      <c r="S23">
+      <c r="T23">
         <v>-53</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <v>-19</v>
       </c>
-      <c r="U23" s="2">
+      <c r="V23" s="2">
         <f t="shared" si="2"/>
         <v>-22.6</v>
       </c>
-      <c r="V23">
-        <v>23.404604941439494</v>
-      </c>
-      <c r="AC23" t="s">
-        <v>64</v>
+      <c r="W23">
+        <v>11.293103005929177</v>
+      </c>
+      <c r="X23">
+        <v>3.02</v>
+      </c>
+      <c r="Y23">
+        <v>-1.41</v>
+      </c>
+      <c r="Z23">
+        <v>0.52</v>
       </c>
     </row>
-    <row r="24" spans="1:29">
+    <row r="24" spans="1:26">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24">
         <v>0</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>3</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>92</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>113</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <f t="shared" si="0"/>
         <v>113</v>
       </c>
-      <c r="H24" s="3">
+      <c r="I24" s="3">
         <v>0</v>
       </c>
-      <c r="I24" s="3">
+      <c r="J24" s="3">
         <v>5.4137943479987002E-2</v>
       </c>
-      <c r="J24" s="3">
+      <c r="K24" s="3">
         <v>1.6602302667196016</v>
       </c>
-      <c r="K24" s="3">
+      <c r="L24" s="3">
         <v>2.0391958710795106</v>
       </c>
-      <c r="L24" s="3">
+      <c r="M24" s="3">
         <f t="shared" si="1"/>
         <v>2.0391958710795106</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>55.414000000000001</v>
       </c>
-      <c r="N24" s="3">
+      <c r="O24" s="3">
         <v>22865</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <v>2.8</v>
       </c>
-      <c r="P24">
+      <c r="Q24">
         <v>-11</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <v>-3</v>
       </c>
-      <c r="R24">
+      <c r="S24">
         <v>0</v>
       </c>
-      <c r="S24">
+      <c r="T24">
         <v>-27</v>
       </c>
-      <c r="T24">
+      <c r="U24">
         <v>-9</v>
       </c>
-      <c r="U24" s="2">
+      <c r="V24" s="2">
         <f t="shared" si="2"/>
         <v>-10</v>
       </c>
-      <c r="V24">
-        <v>18.092186380863229</v>
-      </c>
-      <c r="AC24" t="s">
-        <v>64</v>
+      <c r="W24">
+        <v>8.4769904343151339</v>
+      </c>
+      <c r="X24">
+        <v>2.98</v>
+      </c>
+      <c r="Y24">
+        <v>-1.96</v>
+      </c>
+      <c r="Z24">
+        <v>0.92</v>
       </c>
     </row>
-    <row r="25" spans="1:29">
+    <row r="25" spans="1:26">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25">
         <v>10</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>205</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>675</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>1750</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <f t="shared" si="0"/>
         <v>1740</v>
       </c>
-      <c r="H25" s="3">
+      <c r="I25" s="3">
         <v>0.29108691855388019</v>
       </c>
-      <c r="I25" s="3">
+      <c r="J25" s="3">
         <v>5.9672818303545441</v>
       </c>
-      <c r="J25" s="3">
+      <c r="K25" s="3">
         <v>19.648367002386912</v>
       </c>
-      <c r="K25" s="3">
+      <c r="L25" s="3">
         <v>50.940210746929033</v>
       </c>
-      <c r="L25" s="3">
+      <c r="M25" s="3">
         <f t="shared" si="1"/>
         <v>50.649123828375153</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>34.353999999999999</v>
       </c>
-      <c r="N25" s="3">
+      <c r="O25" s="3">
         <v>4525</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <v>3.62</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
         <v>-24</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <v>-15</v>
       </c>
-      <c r="R25">
+      <c r="S25">
         <v>-17</v>
       </c>
-      <c r="S25">
+      <c r="T25">
         <v>-38</v>
       </c>
-      <c r="T25">
+      <c r="U25">
         <v>-15</v>
       </c>
-      <c r="U25" s="2">
+      <c r="V25" s="2">
         <f t="shared" si="2"/>
         <v>-21.8</v>
       </c>
-      <c r="V25">
-        <v>16.200950512469316</v>
-      </c>
-      <c r="AC25" t="s">
-        <v>64</v>
+      <c r="W25">
+        <v>8.8943091681000794</v>
+      </c>
+      <c r="X25">
+        <v>1.48</v>
+      </c>
+      <c r="Y25">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="Z25">
+        <v>3.45</v>
       </c>
     </row>
-    <row r="26" spans="1:29">
+    <row r="26" spans="1:26">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26">
         <v>3</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>41</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>117</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>226</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <f t="shared" si="0"/>
         <v>223</v>
       </c>
-      <c r="H26" s="3">
+      <c r="I26" s="3">
         <v>4.2085770800892215E-2</v>
       </c>
-      <c r="I26" s="3">
+      <c r="J26" s="3">
         <v>0.57517220094552701</v>
       </c>
-      <c r="J26" s="3">
+      <c r="K26" s="3">
         <v>1.6413450612347964</v>
       </c>
-      <c r="K26" s="3">
+      <c r="L26" s="3">
         <v>3.1704614003338802</v>
       </c>
-      <c r="L26" s="3">
+      <c r="M26" s="3">
         <f t="shared" si="1"/>
         <v>3.1283756295329881</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>71.283000000000001</v>
       </c>
-      <c r="N26" s="3">
+      <c r="O26" s="3">
         <v>156146</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <v>5.07</v>
       </c>
-      <c r="P26">
+      <c r="Q26">
         <v>-9</v>
       </c>
-      <c r="Q26">
+      <c r="R26">
         <v>-3</v>
       </c>
-      <c r="R26">
+      <c r="S26">
         <v>-7</v>
       </c>
-      <c r="S26">
+      <c r="T26">
         <v>-39</v>
       </c>
-      <c r="T26">
+      <c r="U26">
         <v>-17</v>
       </c>
-      <c r="U26" s="2">
+      <c r="V26" s="2">
         <f t="shared" si="2"/>
         <v>-15</v>
       </c>
-      <c r="V26">
-        <v>11.098976360008555</v>
-      </c>
-      <c r="AC26" t="s">
-        <v>61</v>
+      <c r="W26">
+        <v>1.8860865579354273</v>
+      </c>
+      <c r="X26">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="Y26">
+        <v>-3.22</v>
+      </c>
+      <c r="Z26">
+        <v>-4.49</v>
       </c>
     </row>
-    <row r="27" spans="1:29">
+    <row r="27" spans="1:26">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27">
         <v>1</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>42</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>92</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>115</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <f t="shared" si="0"/>
         <v>114</v>
       </c>
-      <c r="H27" s="3">
+      <c r="I27" s="3">
         <v>7.1174377224199281E-2</v>
       </c>
-      <c r="I27" s="3">
+      <c r="J27" s="3">
         <v>2.9893238434163698</v>
       </c>
-      <c r="J27" s="3">
+      <c r="K27" s="3">
         <v>6.5480427046263339</v>
       </c>
-      <c r="K27" s="3">
+      <c r="L27" s="3">
         <v>8.185053380782918</v>
       </c>
-      <c r="L27" s="3">
+      <c r="M27" s="3">
         <f t="shared" si="1"/>
         <v>8.1138790035587185</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>14.05</v>
       </c>
-      <c r="N27" s="3">
+      <c r="O27" s="3">
         <v>6115</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>2.61</v>
       </c>
-      <c r="P27">
+      <c r="Q27">
         <v>-10</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
         <v>-3</v>
       </c>
-      <c r="R27">
+      <c r="S27">
         <v>-20</v>
       </c>
-      <c r="S27">
+      <c r="T27">
         <v>-42</v>
       </c>
-      <c r="T27">
+      <c r="U27">
         <v>-12</v>
       </c>
-      <c r="U27" s="2">
+      <c r="V27" s="2">
         <f t="shared" si="2"/>
         <v>-17.399999999999999</v>
       </c>
-      <c r="V27">
-        <v>11.574105622589343</v>
-      </c>
-      <c r="AC27" t="s">
-        <v>63</v>
+      <c r="W27">
+        <v>3.9614587474659002</v>
+      </c>
+      <c r="X27">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="Y27">
+        <v>-0.78</v>
+      </c>
+      <c r="Z27">
+        <v>-1.27</v>
       </c>
     </row>
-    <row r="28" spans="1:29">
+    <row r="28" spans="1:26">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28">
         <v>50</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>491</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>1541</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>5084</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <f t="shared" si="0"/>
         <v>5034</v>
       </c>
-      <c r="H28" s="3">
+      <c r="I28" s="3">
         <v>0.56003584229390679</v>
       </c>
-      <c r="I28" s="3">
+      <c r="J28" s="3">
         <v>5.4995519713261647</v>
       </c>
-      <c r="J28" s="3">
+      <c r="K28" s="3">
         <v>17.260304659498207</v>
       </c>
-      <c r="K28" s="3">
+      <c r="L28" s="3">
         <v>56.944444444444443</v>
       </c>
-      <c r="L28" s="3">
+      <c r="M28" s="3">
         <f t="shared" si="1"/>
         <v>56.384408602150536</v>
       </c>
-      <c r="M28">
+      <c r="N28">
         <v>89.28</v>
       </c>
-      <c r="N28" s="3">
+      <c r="O28" s="3">
         <v>41908</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>6.07</v>
       </c>
-      <c r="P28">
+      <c r="Q28">
         <v>-20</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <v>-5</v>
       </c>
-      <c r="R28">
+      <c r="S28">
         <v>-10</v>
       </c>
-      <c r="S28">
+      <c r="T28">
         <v>-52</v>
       </c>
-      <c r="T28">
+      <c r="U28">
         <v>-26</v>
       </c>
-      <c r="U28" s="2">
+      <c r="V28" s="2">
         <f t="shared" si="2"/>
         <v>-22.6</v>
       </c>
-      <c r="V28">
-        <v>20.656283078784217</v>
-      </c>
-      <c r="AC28" t="s">
-        <v>63</v>
+      <c r="W28">
+        <v>7.0043853016785116</v>
+      </c>
+      <c r="X28">
+        <v>3.07</v>
+      </c>
+      <c r="Y28">
+        <v>-3.87</v>
+      </c>
+      <c r="Z28">
+        <v>-0.41</v>
       </c>
     </row>
-    <row r="29" spans="1:29">
+    <row r="29" spans="1:26">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29">
         <v>3</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>47</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>128</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>189</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <f t="shared" si="0"/>
         <v>186</v>
       </c>
-      <c r="H29" s="3">
+      <c r="I29" s="3">
         <v>9.6867936712948022E-2</v>
       </c>
-      <c r="I29" s="3">
+      <c r="J29" s="3">
         <v>1.517597675169519</v>
       </c>
-      <c r="J29" s="3">
+      <c r="K29" s="3">
         <v>4.1330319664191153</v>
       </c>
-      <c r="K29" s="3">
+      <c r="L29" s="3">
         <v>6.1026800129157248</v>
       </c>
-      <c r="L29" s="3">
+      <c r="M29" s="3">
         <f t="shared" si="1"/>
         <v>6.0058120762027771</v>
       </c>
-      <c r="M29">
+      <c r="N29">
         <v>30.97</v>
       </c>
-      <c r="N29" s="3">
+      <c r="O29" s="3">
         <v>23348</v>
       </c>
-      <c r="O29">
+      <c r="P29">
         <v>2.98</v>
       </c>
-      <c r="P29">
+      <c r="Q29">
         <v>-9</v>
       </c>
-      <c r="Q29">
+      <c r="R29">
         <v>-2</v>
       </c>
-      <c r="R29">
+      <c r="S29">
         <v>-5</v>
       </c>
-      <c r="S29">
+      <c r="T29">
         <v>-38</v>
       </c>
-      <c r="T29">
+      <c r="U29">
         <v>-14</v>
       </c>
-      <c r="U29" s="2">
+      <c r="V29" s="2">
         <f t="shared" si="2"/>
         <v>-13.6</v>
       </c>
-      <c r="V29">
-        <v>12.530378584672992</v>
-      </c>
-      <c r="AC29" t="s">
-        <v>63</v>
+      <c r="W29">
+        <v>5.1693099785774717</v>
+      </c>
+      <c r="X29">
+        <v>4.92</v>
+      </c>
+      <c r="Y29">
+        <v>-0.06</v>
+      </c>
+      <c r="Z29">
+        <v>0.71</v>
       </c>
     </row>
-    <row r="30" spans="1:29">
+    <row r="30" spans="1:26">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30">
         <v>3</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>62</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>244</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>363</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <f t="shared" si="0"/>
         <v>360</v>
       </c>
-      <c r="H30" s="3">
+      <c r="I30" s="3">
         <v>0.10886921178690666</v>
       </c>
-      <c r="I30" s="3">
+      <c r="J30" s="3">
         <v>2.2499637102627377</v>
       </c>
-      <c r="J30" s="3">
+      <c r="K30" s="3">
         <v>8.8546958920017413</v>
       </c>
-      <c r="K30" s="3">
+      <c r="L30" s="3">
         <v>13.173174626215706</v>
       </c>
-      <c r="L30" s="3">
+      <c r="M30" s="3">
         <f t="shared" si="1"/>
         <v>13.0643054144288</v>
       </c>
-      <c r="M30">
+      <c r="N30">
         <v>27.556000000000001</v>
       </c>
-      <c r="N30" s="3">
+      <c r="O30" s="3">
         <v>34454</v>
       </c>
-      <c r="O30">
+      <c r="P30">
         <v>3.17</v>
       </c>
-      <c r="P30">
+      <c r="Q30">
         <v>-12</v>
       </c>
-      <c r="Q30">
+      <c r="R30">
         <v>1</v>
       </c>
-      <c r="R30">
+      <c r="S30">
         <v>-15</v>
       </c>
-      <c r="S30">
+      <c r="T30">
         <v>-35</v>
       </c>
-      <c r="T30">
+      <c r="U30">
         <v>-14</v>
       </c>
-      <c r="U30" s="2">
+      <c r="V30" s="2">
         <f t="shared" si="2"/>
         <v>-15</v>
       </c>
-      <c r="V30">
-        <v>17.985745045746683</v>
-      </c>
-      <c r="AC30" t="s">
-        <v>63</v>
+      <c r="W30">
+        <v>6.848867854744638</v>
+      </c>
+      <c r="X30">
+        <v>4.37</v>
+      </c>
+      <c r="Y30">
+        <v>-2.39</v>
+      </c>
+      <c r="Z30">
+        <v>-0.11</v>
       </c>
     </row>
-    <row r="31" spans="1:29">
+    <row r="31" spans="1:26">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31">
         <v>2</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>45</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>339</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>1109</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <f t="shared" si="0"/>
         <v>1107</v>
       </c>
-      <c r="H31" s="3">
+      <c r="I31" s="3">
         <v>7.9088895919012969E-2</v>
       </c>
-      <c r="I31" s="3">
+      <c r="J31" s="3">
         <v>1.7795001581777918</v>
       </c>
-      <c r="J31" s="3">
+      <c r="K31" s="3">
         <v>13.405567858272699</v>
       </c>
-      <c r="K31" s="3">
+      <c r="L31" s="3">
         <v>43.854792787092691</v>
       </c>
-      <c r="L31" s="3">
+      <c r="M31" s="3">
         <f t="shared" si="1"/>
         <v>43.775703891173677</v>
       </c>
-      <c r="M31">
+      <c r="N31">
         <v>25.288</v>
       </c>
-      <c r="N31" s="3">
+      <c r="O31" s="3">
         <v>29557</v>
       </c>
-      <c r="O31">
+      <c r="P31">
         <v>5.57</v>
       </c>
-      <c r="P31">
+      <c r="Q31">
         <v>-30</v>
       </c>
-      <c r="Q31">
+      <c r="R31">
         <v>-9</v>
       </c>
-      <c r="R31">
+      <c r="S31">
         <v>-20</v>
       </c>
-      <c r="S31">
+      <c r="T31">
         <v>-40</v>
       </c>
-      <c r="T31">
+      <c r="U31">
         <v>-24</v>
       </c>
-      <c r="U31" s="2">
+      <c r="V31" s="2">
         <f t="shared" si="2"/>
         <v>-24.6</v>
       </c>
-      <c r="V31">
-        <v>24.202092398443035</v>
-      </c>
-      <c r="AC31" t="s">
-        <v>63</v>
+      <c r="W31">
+        <v>13.106515506803095</v>
+      </c>
+      <c r="X31">
+        <v>4.28</v>
+      </c>
+      <c r="Y31">
+        <v>-3.89</v>
+      </c>
+      <c r="Z31">
+        <v>-3.16</v>
       </c>
     </row>
-    <row r="32" spans="1:29">
+    <row r="32" spans="1:26">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32">
         <v>8</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>148</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>567</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>726</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <f t="shared" si="0"/>
         <v>718</v>
       </c>
-      <c r="H32" s="3">
+      <c r="I32" s="3">
         <v>0.14548628791736379</v>
       </c>
-      <c r="I32" s="3">
+      <c r="J32" s="3">
         <v>2.6914963264712299</v>
       </c>
-      <c r="J32" s="3">
+      <c r="K32" s="3">
         <v>10.311340656143159</v>
       </c>
-      <c r="K32" s="3">
+      <c r="L32" s="3">
         <v>13.202880628500765</v>
       </c>
-      <c r="L32" s="3">
+      <c r="M32" s="3">
         <f t="shared" si="1"/>
         <v>13.0573943405834</v>
       </c>
-      <c r="M32">
+      <c r="N32">
         <v>54.988</v>
       </c>
-      <c r="N32" s="3">
+      <c r="O32" s="3">
         <v>39411</v>
       </c>
-      <c r="O32">
+      <c r="P32">
         <v>5.22</v>
       </c>
-      <c r="P32">
+      <c r="Q32">
         <v>-7</v>
       </c>
-      <c r="Q32">
+      <c r="R32">
         <v>6</v>
       </c>
-      <c r="R32">
+      <c r="S32">
         <v>-2</v>
       </c>
-      <c r="S32">
+      <c r="T32">
         <v>-31</v>
       </c>
-      <c r="T32">
+      <c r="U32">
         <v>-22</v>
       </c>
-      <c r="U32" s="2">
+      <c r="V32" s="2">
         <f t="shared" si="2"/>
         <v>-11.2</v>
       </c>
-      <c r="V32">
-        <v>29.476906416315135</v>
-      </c>
-      <c r="AC32" t="s">
-        <v>61</v>
+      <c r="W32">
+        <v>15.535464856330181</v>
+      </c>
+      <c r="X32">
+        <v>3.9</v>
+      </c>
+      <c r="Y32">
+        <v>-4.91</v>
+      </c>
+      <c r="Z32">
+        <v>-5.5</v>
       </c>
     </row>
-    <row r="33" spans="1:29">
+    <row r="33" spans="1:26">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
       </c>
-      <c r="C33">
+      <c r="C33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33">
         <v>5</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>150</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>982</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>2049</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <f t="shared" si="0"/>
         <v>2044</v>
       </c>
-      <c r="H33" s="3">
+      <c r="I33" s="3">
         <v>5.8357357112011107E-2</v>
       </c>
-      <c r="I33" s="3">
+      <c r="J33" s="3">
         <v>1.7507207133603333</v>
       </c>
-      <c r="J33" s="3">
+      <c r="K33" s="3">
         <v>11.461384936798982</v>
       </c>
-      <c r="K33" s="3">
+      <c r="L33" s="3">
         <v>23.914844944502153</v>
       </c>
-      <c r="L33" s="3">
+      <c r="M33" s="3">
         <f t="shared" si="1"/>
         <v>23.856487587390141</v>
       </c>
-      <c r="M33">
+      <c r="N33">
         <v>85.679000000000002</v>
       </c>
-      <c r="N33" s="3">
+      <c r="O33" s="3">
         <v>56867</v>
       </c>
-      <c r="O33">
+      <c r="P33">
         <v>3.86</v>
       </c>
-      <c r="P33">
+      <c r="Q33">
         <v>-13</v>
       </c>
-      <c r="Q33">
+      <c r="R33">
         <v>-2</v>
       </c>
-      <c r="R33">
+      <c r="S33">
         <v>1</v>
       </c>
-      <c r="S33">
+      <c r="T33">
         <v>-41</v>
       </c>
-      <c r="T33">
+      <c r="U33">
         <v>-22</v>
       </c>
-      <c r="U33" s="2">
+      <c r="V33" s="2">
         <f t="shared" si="2"/>
         <v>-15.4</v>
       </c>
-      <c r="V33">
-        <v>14.182387804904323</v>
-      </c>
-      <c r="AC33" t="s">
-        <v>61</v>
+      <c r="W33">
+        <v>4.4753519631805041</v>
+      </c>
+      <c r="X33">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="Y33">
+        <v>-1.37</v>
+      </c>
+      <c r="Z33">
+        <v>-2.2999999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:29">
+    <row r="34" spans="1:26">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
       </c>
-      <c r="C34">
+      <c r="C34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34">
         <v>19</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>117</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>409</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>1551</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <f t="shared" si="0"/>
         <v>1532</v>
       </c>
-      <c r="H34" s="3">
+      <c r="I34" s="3">
         <v>0.1292209337912742</v>
       </c>
-      <c r="I34" s="3">
+      <c r="J34" s="3">
         <v>0.79572890808310948</v>
       </c>
-      <c r="J34" s="3">
+      <c r="K34" s="3">
         <v>2.781650627401639</v>
       </c>
-      <c r="K34" s="3">
+      <c r="L34" s="3">
         <v>10.548508858435067</v>
       </c>
-      <c r="L34" s="3">
+      <c r="M34" s="3">
         <f t="shared" si="1"/>
         <v>10.419287924643793</v>
       </c>
-      <c r="M34">
+      <c r="N34">
         <v>147.035</v>
       </c>
-      <c r="N34" s="3">
+      <c r="O34" s="3">
         <v>108407</v>
       </c>
-      <c r="O34">
+      <c r="P34">
         <v>4.7300000000000004</v>
       </c>
-      <c r="P34">
+      <c r="Q34">
         <v>-19</v>
       </c>
-      <c r="Q34">
+      <c r="R34">
         <v>-7</v>
       </c>
-      <c r="R34">
+      <c r="S34">
         <v>-16</v>
       </c>
-      <c r="S34">
+      <c r="T34">
         <v>-36</v>
       </c>
-      <c r="T34">
+      <c r="U34">
         <v>-22</v>
       </c>
-      <c r="U34" s="2">
+      <c r="V34" s="2">
         <f t="shared" si="2"/>
         <v>-20</v>
       </c>
-      <c r="V34">
-        <v>25.194644712605459</v>
-      </c>
-      <c r="AC34" t="s">
-        <v>61</v>
+      <c r="W34">
+        <v>8.6667385815639122</v>
+      </c>
+      <c r="X34">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="Y34">
+        <v>-2.37</v>
+      </c>
+      <c r="Z34">
+        <v>-4.75</v>
       </c>
     </row>
-    <row r="35" spans="1:29">
+    <row r="35" spans="1:26">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>34</v>
       </c>
-      <c r="C35">
+      <c r="C35" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35">
         <v>23</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>95</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>236</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>313</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <f t="shared" si="0"/>
         <v>290</v>
       </c>
-      <c r="H35" s="3">
+      <c r="I35" s="3">
         <v>0.5924323210468021</v>
       </c>
-      <c r="I35" s="3">
+      <c r="J35" s="3">
         <v>2.447003065193313</v>
       </c>
-      <c r="J35" s="3">
+      <c r="K35" s="3">
         <v>6.0788707724802311</v>
       </c>
-      <c r="K35" s="3">
+      <c r="L35" s="3">
         <v>8.0622311516369169</v>
       </c>
-      <c r="L35" s="3">
+      <c r="M35" s="3">
         <f t="shared" si="1"/>
         <v>7.4697988305901148</v>
       </c>
-      <c r="M35">
+      <c r="N35">
         <v>38.823</v>
       </c>
-      <c r="N35" s="3">
+      <c r="O35" s="3">
         <v>34728</v>
       </c>
-      <c r="O35">
+      <c r="P35">
         <v>3.38</v>
       </c>
-      <c r="P35">
+      <c r="Q35">
         <v>-24</v>
       </c>
-      <c r="Q35">
+      <c r="R35">
         <v>-17</v>
       </c>
-      <c r="R35">
+      <c r="S35">
         <v>-34</v>
       </c>
-      <c r="S35">
+      <c r="T35">
         <v>-57</v>
       </c>
-      <c r="T35">
+      <c r="U35">
         <v>-32</v>
       </c>
-      <c r="U35" s="2">
+      <c r="V35" s="2">
         <f t="shared" si="2"/>
         <v>-32.799999999999997</v>
       </c>
-      <c r="V35">
-        <v>23.30805387064655</v>
-      </c>
-      <c r="AC35" t="s">
-        <v>62</v>
+      <c r="W35">
+        <v>18.970781542641252</v>
+      </c>
+      <c r="X35">
+        <v>-0.17</v>
+      </c>
+      <c r="Y35">
+        <v>-6.74</v>
+      </c>
+      <c r="Z35">
+        <v>-6.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>